<commit_message>
EPBDS-4790 [Web Services] Incorrect result of running test table in case project has depended module
</commit_message>
<xml_diff>
--- a/WSFrontend/org.openl.rules.ruleservice/test-resources/DomainSharingTest/project2/Module2_1.xlsx
+++ b/WSFrontend/org.openl.rules.ruleservice/test-resources/DomainSharingTest/project2/Module2_1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>Environment</t>
   </si>
@@ -74,6 +74,15 @@
   </si>
   <si>
     <t>Data TestBean beans2</t>
+  </si>
+  <si>
+    <t>properties</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>0.0.2</t>
   </si>
 </sst>
 </file>
@@ -199,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -208,6 +217,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -217,9 +229,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -286,9 +299,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -326,7 +339,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -398,7 +411,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -572,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G23"/>
+  <dimension ref="B3:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:G4"/>
+      <selection activeCell="B23" sqref="B23:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,137 +602,194 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="F4" s="8" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="F5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="9"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F6" s="4" t="s">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G7" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="F7" s="6" t="s">
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="F8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G8" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="10" t="s">
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="10" t="s">
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="10" t="s">
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="10" t="s">
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="10" t="s">
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="10" t="s">
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="8" t="s">
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="9"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
+      <c r="C26" s="10"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
     <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B15:D15"/>
     <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B10:D10"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B24:D24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>